<commit_message>
Updated communication protocol - included fluidics and sorted alphabetically
</commit_message>
<xml_diff>
--- a/doc/data packet structure.xlsx
+++ b/doc/data packet structure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkiselev\Documents\dev\sync_device\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ECB9A70-B195-4AAB-B538-2A64807A377B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF1AA55B-FB9D-49CD-8068-B8BD73422F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{48FB7E95-C391-4754-94A5-34D8116DC883}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28440" xr2:uid="{48FB7E95-C391-4754-94A5-34D8116DC883}"/>
   </bookViews>
   <sheets>
     <sheet name="Data packet format" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
   <si>
     <r>
       <t xml:space="preserve">uint8       </t>
@@ -854,6 +854,61 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> (NOT IMPLEMENTED)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">uint8        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'F'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">uint32                                </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>fluidics_frame</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Set frame for micro</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>luidic trigger</t>
     </r>
   </si>
 </sst>
@@ -1149,13 +1204,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1170,7 +1225,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1179,18 +1234,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1233,7 +1281,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1248,8 +1296,17 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1267,18 +1324,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1304,9 +1349,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1344,7 +1389,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1450,7 +1495,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1592,7 +1637,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1600,46 +1645,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6FE895D-0C3B-46E0-B798-2A07ED6015B0}">
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="2" max="6" width="6.44140625" customWidth="1"/>
-    <col min="7" max="7" width="0.88671875" customWidth="1"/>
-    <col min="8" max="8" width="26.44140625" customWidth="1"/>
-    <col min="9" max="9" width="6.44140625" customWidth="1"/>
-    <col min="10" max="10" width="6.33203125" customWidth="1"/>
+    <col min="2" max="6" width="6.42578125" customWidth="1"/>
+    <col min="7" max="7" width="0.85546875" customWidth="1"/>
+    <col min="8" max="8" width="26.7109375" customWidth="1"/>
+    <col min="9" max="9" width="6.42578125" customWidth="1"/>
+    <col min="10" max="10" width="6.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="23" t="s">
+    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="20" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="35">
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="32">
         <v>0</v>
       </c>
-      <c r="C2" s="35">
+      <c r="C2" s="32">
         <v>1</v>
       </c>
-      <c r="D2" s="35">
+      <c r="D2" s="32">
         <v>2</v>
       </c>
-      <c r="E2" s="35">
+      <c r="E2" s="32">
         <v>3</v>
       </c>
-      <c r="F2" s="35">
+      <c r="F2" s="32">
         <v>4</v>
       </c>
-      <c r="G2" s="11"/>
-    </row>
-    <row r="3" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:10" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8"/>
       <c r="B3" s="7" t="s">
         <v>3</v>
@@ -1648,126 +1692,124 @@
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="17" t="s">
+      <c r="G3" s="11"/>
+      <c r="H3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="17" t="s">
+      <c r="I3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="17" t="s">
+      <c r="J3" s="14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="45" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" s="21" t="s">
+    <row r="4" spans="1:10" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="40" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="I5" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="J5" s="21" t="s">
+    <row r="5" spans="1:10" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="I5" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="30" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="45" t="s">
-        <v>7</v>
+    <row r="6" spans="1:10" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="35" t="s">
+        <v>40</v>
       </c>
       <c r="C6" s="40" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D6" s="41"/>
       <c r="E6" s="41"/>
       <c r="F6" s="42"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="18" t="s">
+      <c r="G6" s="12"/>
+      <c r="H6" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="I7" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="J6" s="21" t="s">
+      <c r="J7" s="18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="46" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="I7" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="J7" s="33" t="s">
+    <row r="8" spans="1:10" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="I8" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" s="30" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="I8" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="J8" s="21" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="45" t="s">
+    <row r="9" spans="1:10" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="35" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="40" t="s">
@@ -1776,209 +1818,234 @@
       <c r="D9" s="41"/>
       <c r="E9" s="41"/>
       <c r="F9" s="42"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="18" t="s">
+      <c r="G9" s="12"/>
+      <c r="H9" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="I9" s="18" t="s">
+      <c r="I9" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="J9" s="21" t="s">
+      <c r="J9" s="18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="45" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="I10" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="J10" s="21" t="s">
+    <row r="10" spans="1:10" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="J10" s="18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="45" t="s">
+    <row r="11" spans="1:10" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="44"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="18" t="s">
+      <c r="C11" s="34"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="I11" s="18" t="s">
+      <c r="I11" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="J11" s="21" t="s">
+      <c r="J11" s="18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="45" t="s">
+    <row r="12" spans="1:10" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="28"/>
+      <c r="C12" s="25"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="4"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="18" t="s">
+      <c r="G12" s="12"/>
+      <c r="H12" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="I12" s="18" t="s">
+      <c r="I12" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="J12" s="21" t="s">
+      <c r="J12" s="18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="45" t="s">
+    <row r="13" spans="1:10" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="23" t="s">
         <v>4</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="4"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="18" t="s">
+      <c r="G13" s="12"/>
+      <c r="H13" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="I13" s="29" t="s">
+      <c r="I13" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="J13" s="20" t="s">
+      <c r="J13" s="17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="45" t="s">
+    <row r="14" spans="1:10" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="J14" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="43" t="s">
+      <c r="C15" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="34" t="s">
+      <c r="D15" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="18" t="s">
+      <c r="E15" s="5"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="29" t="s">
+      <c r="I15" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="J14" s="21"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="22"/>
-      <c r="B15" s="35">
+      <c r="J15" s="18"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="19"/>
+      <c r="B16" s="32">
         <v>0</v>
       </c>
-      <c r="C15" s="36">
+      <c r="C16" s="32">
         <v>1</v>
       </c>
-      <c r="D15" s="35">
+      <c r="D16" s="32">
         <v>2</v>
       </c>
-      <c r="E15" s="35">
+      <c r="E16" s="32">
         <v>3</v>
       </c>
-      <c r="F15" s="35">
+      <c r="F16" s="32">
         <v>4</v>
       </c>
-      <c r="G15" s="14"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="1"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="14"/>
-    </row>
-    <row r="17" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B17" s="2" t="s">
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="2:14" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>21</v>
       </c>
-      <c r="N20" s="30"/>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
+      <c r="N21" s="27"/>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B23" s="2" t="s">
+    <row r="23" spans="2:14" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B24" s="19" t="s">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B25" s="16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
         <v>22</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C14:F14"/>
     <mergeCell ref="C7:F7"/>
-    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C9:F9"/>
     <mergeCell ref="C6:F6"/>
     <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C8:F8"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="110" fitToWidth="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed typo in documentation re fluidics trigger
</commit_message>
<xml_diff>
--- a/doc/data packet structure.xlsx
+++ b/doc/data packet structure.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkiselev\Documents\dev\sync_device\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF1AA55B-FB9D-49CD-8068-B8BD73422F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E31C37DD-A555-4F8E-AB28-B342E45043C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28440" xr2:uid="{48FB7E95-C391-4754-94A5-34D8116DC883}"/>
   </bookViews>
@@ -874,7 +874,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">uint32                                </t>
+      <t xml:space="preserve">int32                                </t>
     </r>
     <r>
       <rPr>
@@ -908,7 +908,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>luidic trigger</t>
+      <t>luidic trigger (-1 means no trigger)</t>
     </r>
   </si>
 </sst>
@@ -1648,7 +1648,7 @@
   <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>